<commit_message>
Corriendo plantilla de cargue de ejemplo
</commit_message>
<xml_diff>
--- a/App/RegistroAsistenciasSMART.Web/Formato/PlantillaEjemplo.xlsx
+++ b/App/RegistroAsistenciasSMART.Web/Formato/PlantillaEjemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuentes\FuentesSMART\AsistenciasV2\App\RegistroAsistenciasSMART.Web\Formato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D69E70-D26B-4478-9120-D5EBBBF381CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D855E9F-E8AF-4D21-A03B-32FC1CBC3A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01196104-56FC-4D66-A5D6-1A230B06E7A5}"/>
   </bookViews>
@@ -60,12 +60,6 @@
     <t>CÉDULA DEL JEFE INMEDIATO</t>
   </si>
   <si>
-    <t>HORA DE ENTRADA L-V</t>
-  </si>
-  <si>
-    <t>HORA DE SALIDA L-V</t>
-  </si>
-  <si>
     <t>HORA DE SALIDA SÁBADOS</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>HORA DE SALIDA VIERNES</t>
+  </si>
+  <si>
+    <t>HORA DE SALIDA L-J</t>
+  </si>
+  <si>
+    <t>HORA DE ENTRADA L-J</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,22 +515,22 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -538,22 +538,22 @@
         <v>102397458</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="I2" s="4">
         <v>0.3125</v>

</xml_diff>